<commit_message>
Updated Excel sheet and added methods in ElementAction and Enhanced invalidLogin Test case
</commit_message>
<xml_diff>
--- a/src/test/java/utilities/testdata.xlsx
+++ b/src/test/java/utilities/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t xml:space="preserve">VALID CREDENTIALS</t>
   </si>
@@ -37,13 +37,22 @@
     <t xml:space="preserve">admin123</t>
   </si>
   <si>
+    <t xml:space="preserve">vj2805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vishalj2805</t>
+  </si>
+  <si>
     <t xml:space="preserve">INVALID CREDENTIALS</t>
   </si>
   <si>
     <t xml:space="preserve">vishalj</t>
   </si>
   <si>
-    <t xml:space="preserve">vishalj2805</t>
+    <t xml:space="preserve">vsj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vsj2805</t>
   </si>
 </sst>
 </file>
@@ -321,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -355,10 +364,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -371,10 +387,18 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced project and Added Test Case Verify Menu Items
</commit_message>
<xml_diff>
--- a/src/test/java/utilities/testdata.xlsx
+++ b/src/test/java/utilities/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t xml:space="preserve">VALID CREDENTIALS</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vj2805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vishalj28051</t>
   </si>
   <si>
     <t xml:space="preserve">INVALID CREDENTIALS</t>
@@ -333,10 +327,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -367,25 +361,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -396,14 +390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>